<commit_message>
Familiar Widget pilot handles the new FM declaration and the merge of Universes (highcharts + amcharts)
</commit_message>
<xml_diff>
--- a/src/main/resources/amcharts.xlsx
+++ b/src/main/resources/amcharts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="4500" windowWidth="28100" windowHeight="13840" tabRatio="500"/>
+    <workbookView xWindow="4480" yWindow="4500" windowWidth="33180" windowHeight="19300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="amcharts.csv" sheetId="1" r:id="rId1"/>
@@ -107,33 +107,6 @@
     <t>Extremum</t>
   </si>
   <si>
-    <t>2D_i</t>
-  </si>
-  <si>
-    <t>2D+_i</t>
-  </si>
-  <si>
-    <t>3D_i</t>
-  </si>
-  <si>
-    <t>3D+_i</t>
-  </si>
-  <si>
-    <t>1D_o</t>
-  </si>
-  <si>
-    <t>2D_o</t>
-  </si>
-  <si>
-    <t>2D+_o</t>
-  </si>
-  <si>
-    <t>3D_o</t>
-  </si>
-  <si>
-    <t>3D+_o</t>
-  </si>
-  <si>
     <t>Histogram</t>
   </si>
   <si>
@@ -143,7 +116,34 @@
     <t>ScatterPlot</t>
   </si>
   <si>
-    <t>1D+_o</t>
+    <t>"2D_i"</t>
+  </si>
+  <si>
+    <t>"2D+_i"</t>
+  </si>
+  <si>
+    <t>"3D_i"</t>
+  </si>
+  <si>
+    <t>"3D+_i"</t>
+  </si>
+  <si>
+    <t>"1D_o"</t>
+  </si>
+  <si>
+    <t>"2D_o"</t>
+  </si>
+  <si>
+    <t>"2D+_o"</t>
+  </si>
+  <si>
+    <t>"3D_o"</t>
+  </si>
+  <si>
+    <t>"3D+_o"</t>
+  </si>
+  <si>
+    <t>"1D+_o"</t>
   </si>
 </sst>
 </file>
@@ -464,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V26"/>
+  <dimension ref="A1:T26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+      <selection sqref="A1:T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +476,7 @@
     <col min="11" max="13" width="10.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -512,19 +512,19 @@
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>8</v>
@@ -536,7 +536,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -598,7 +598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -660,7 +660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -722,7 +722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -784,7 +784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -846,7 +846,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -908,7 +908,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -970,7 +970,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -1093,9 +1093,8 @@
       <c r="T10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="V10" s="2"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1219,7 +1218,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1281,7 +1280,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1404,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1469,7 +1468,7 @@
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
@@ -1531,7 +1530,7 @@
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
@@ -1593,7 +1592,7 @@
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
@@ -1655,7 +1654,7 @@
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
@@ -1717,7 +1716,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
@@ -1841,7 +1840,7 @@
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
@@ -1903,7 +1902,7 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
@@ -1965,7 +1964,7 @@
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
@@ -2027,7 +2026,7 @@
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Familiar does not scale when merging 34 fms AND asFM lose the constraints AND merge(merge(fm_1*),merge(fm_2*)) lose some constraints too -> I'm sad
</commit_message>
<xml_diff>
--- a/src/main/resources/amcharts.xlsx
+++ b/src/main/resources/amcharts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4480" yWindow="4500" windowWidth="33180" windowHeight="19300" tabRatio="500"/>
+    <workbookView xWindow="56440" yWindow="9900" windowWidth="34860" windowHeight="17120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="amcharts.csv" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="49">
   <si>
     <t>Pie Chart</t>
   </si>
@@ -116,34 +116,61 @@
     <t>ScatterPlot</t>
   </si>
   <si>
-    <t>"2D_i"</t>
-  </si>
-  <si>
-    <t>"2D+_i"</t>
-  </si>
-  <si>
-    <t>"3D_i"</t>
-  </si>
-  <si>
-    <t>"3D+_i"</t>
-  </si>
-  <si>
-    <t>"1D_o"</t>
-  </si>
-  <si>
-    <t>"2D_o"</t>
-  </si>
-  <si>
-    <t>"2D+_o"</t>
-  </si>
-  <si>
-    <t>"3D_o"</t>
-  </si>
-  <si>
-    <t>"3D+_o"</t>
-  </si>
-  <si>
-    <t>"1D+_o"</t>
+    <t>Concern</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>MultiSet Line Chart</t>
+  </si>
+  <si>
+    <t>MultiSet Step Chart</t>
+  </si>
+  <si>
+    <t>MultiSet Bar Chart</t>
+  </si>
+  <si>
+    <t>MultiSet Bubble Chart</t>
+  </si>
+  <si>
+    <t>MultiSet ScatterPlot</t>
+  </si>
+  <si>
+    <t>MultiSet Radar Chart</t>
+  </si>
+  <si>
+    <t>2D_i</t>
+  </si>
+  <si>
+    <t>2D+_i</t>
+  </si>
+  <si>
+    <t>3D_i</t>
+  </si>
+  <si>
+    <t>3D+_i</t>
+  </si>
+  <si>
+    <t>1D_o</t>
+  </si>
+  <si>
+    <t>1D+_o</t>
+  </si>
+  <si>
+    <t>2D_o</t>
+  </si>
+  <si>
+    <t>2D+_o</t>
+  </si>
+  <si>
+    <t>3D_o</t>
+  </si>
+  <si>
+    <t>3D+_o</t>
   </si>
 </sst>
 </file>
@@ -179,12 +206,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -464,96 +494,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:T26"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" customWidth="1"/>
-    <col min="11" max="13" width="10.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="11" width="9" customWidth="1"/>
+    <col min="12" max="13" width="9" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10" style="2" customWidth="1"/>
+    <col min="15" max="16" width="9" customWidth="1"/>
+    <col min="17" max="18" width="9.6640625" customWidth="1"/>
+    <col min="19" max="21" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:21" ht="64" x14ac:dyDescent="0.2">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="U1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>12</v>
@@ -565,7 +600,7 @@
         <v>12</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
@@ -577,39 +612,42 @@
         <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="U2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
@@ -618,13 +656,13 @@
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>12</v>
@@ -639,13 +677,13 @@
         <v>12</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>12</v>
@@ -654,19 +692,22 @@
         <v>12</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
@@ -674,22 +715,22 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>11</v>
@@ -698,13 +739,13 @@
         <v>11</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>11</v>
@@ -713,22 +754,25 @@
         <v>11</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="U4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
@@ -783,14 +827,17 @@
       <c r="T5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="U5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
@@ -845,14 +892,17 @@
       <c r="T6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="U6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
@@ -884,7 +934,7 @@
         <v>12</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>11</v>
@@ -893,7 +943,7 @@
         <v>11</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>12</v>
@@ -907,19 +957,22 @@
       <c r="T7" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="U7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
@@ -931,10 +984,10 @@
         <v>12</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>12</v>
@@ -969,14 +1022,17 @@
       <c r="T8" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="U8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1005,7 +1061,7 @@
         <v>12</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>11</v>
@@ -1023,27 +1079,30 @@
         <v>11</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
@@ -1085,22 +1144,25 @@
         <v>11</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="U10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
@@ -1132,10 +1194,10 @@
         <v>12</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O11" s="2" t="s">
         <v>12</v>
@@ -1155,19 +1217,22 @@
       <c r="T11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="U11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
@@ -1188,13 +1253,13 @@
         <v>11</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N12" s="2" t="s">
         <v>11</v>
@@ -1212,19 +1277,22 @@
         <v>11</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T12" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="U12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1241,10 +1309,10 @@
         <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>11</v>
@@ -1265,33 +1333,36 @@
         <v>11</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q13" s="2" t="s">
         <v>12</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>12</v>
@@ -1306,7 +1377,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>11</v>
@@ -1333,27 +1404,30 @@
         <v>11</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="U14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
@@ -1374,16 +1448,16 @@
         <v>11</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L15" s="2" t="s">
         <v>12</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O15" s="2" t="s">
         <v>12</v>
@@ -1403,19 +1477,22 @@
       <c r="T15" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="U15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -1424,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>12</v>
@@ -1436,7 +1513,7 @@
         <v>12</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>11</v>
@@ -1451,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>12</v>
@@ -1460,18 +1537,21 @@
         <v>12</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T16" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>11</v>
+      <c r="U16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -1480,60 +1560,63 @@
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>12</v>
+      <c r="B18" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>12</v>
@@ -1542,31 +1625,31 @@
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N18" s="2" t="s">
         <v>12</v>
@@ -1578,154 +1661,163 @@
         <v>12</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S19" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>11</v>
+      <c r="B21" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>12</v>
@@ -1767,21 +1859,24 @@
         <v>12</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
@@ -1835,51 +1930,54 @@
         <v>12</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>12</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>12</v>
@@ -1899,13 +1997,16 @@
       <c r="T23" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>12</v>
+      <c r="U23" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>12</v>
@@ -1914,31 +2015,31 @@
         <v>12</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N24" s="2" t="s">
         <v>12</v>
@@ -1961,13 +2062,16 @@
       <c r="T24" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>12</v>
+      <c r="U24" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>12</v>
@@ -2003,16 +2107,16 @@
         <v>12</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R25" s="2" t="s">
         <v>12</v>
@@ -2023,13 +2127,16 @@
       <c r="T25" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>12</v>
+      <c r="U25" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>12</v>
@@ -2068,21 +2175,24 @@
         <v>12</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="S26" s="2" t="s">
         <v>12</v>
       </c>
       <c r="T26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="U26" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>